<commit_message>
Green for in the bag
</commit_message>
<xml_diff>
--- a/Hardware/Electronics/Classification and Control Board/BoM.xlsx
+++ b/Hardware/Electronics/Classification and Control Board/BoM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Willie\Documents\Uni\Newcastle\4 Fourth Year\1 Final Year Project\trunk\Hardware\Electronics\Classification and Control Board\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908BE73D-47FD-42B8-8427-33EE72246B27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF4F779-F393-4102-82CA-6B0C772E8C28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -830,7 +830,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="170" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -862,12 +862,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -884,7 +890,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -893,10 +899,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1181,8 +1188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:K96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H102" sqref="H102"/>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1227,7 +1234,7 @@
       </c>
     </row>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>9</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1243,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="G2">
-        <f>1-F2</f>
+        <f t="shared" ref="G2:G33" si="0">1-F2</f>
         <v>0</v>
       </c>
       <c r="H2" t="s">
@@ -1260,7 +1267,7 @@
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>30</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1276,7 +1283,7 @@
         <v>1</v>
       </c>
       <c r="G3">
-        <f>1-F3</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H3" t="s">
@@ -1293,7 +1300,7 @@
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1309,7 +1316,7 @@
         <v>1</v>
       </c>
       <c r="G4">
-        <f>1-F4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H4" t="s">
@@ -1326,7 +1333,7 @@
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1342,7 +1349,7 @@
         <v>1</v>
       </c>
       <c r="G5">
-        <f>1-F5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H5" t="s">
@@ -1359,7 +1366,7 @@
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -1375,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="G6">
-        <f>1-F6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6" t="s">
@@ -1392,7 +1399,7 @@
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>27</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -1408,7 +1415,7 @@
         <v>1</v>
       </c>
       <c r="G7">
-        <f>1-F7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H7" t="s">
@@ -1425,7 +1432,7 @@
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>33</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -1441,7 +1448,7 @@
         <v>1</v>
       </c>
       <c r="G8">
-        <f>1-F8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H8" t="s">
@@ -1458,7 +1465,7 @@
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1474,7 +1481,7 @@
         <v>1</v>
       </c>
       <c r="G9">
-        <f>1-F9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H9" t="s">
@@ -1491,7 +1498,7 @@
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -1507,7 +1514,7 @@
         <v>1</v>
       </c>
       <c r="G10">
-        <f>1-F10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H10" t="s">
@@ -1524,7 +1531,7 @@
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="B11" s="6" t="s">
         <v>7</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1540,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="G11">
-        <f>1-F11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H11" t="s">
@@ -1557,7 +1564,7 @@
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="B12" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1573,7 +1580,7 @@
         <v>1</v>
       </c>
       <c r="G12">
-        <f>1-F12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H12" t="s">
@@ -1590,7 +1597,7 @@
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -1606,7 +1613,7 @@
         <v>1</v>
       </c>
       <c r="G13">
-        <f>1-F13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" t="s">
@@ -1623,7 +1630,7 @@
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -1639,7 +1646,7 @@
         <v>1</v>
       </c>
       <c r="G14">
-        <f>1-F14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H14" t="s">
@@ -1656,7 +1663,7 @@
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="B15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -1672,7 +1679,7 @@
         <v>1</v>
       </c>
       <c r="G15">
-        <f>1-F15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H15" t="s">
@@ -1689,7 +1696,7 @@
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="B16" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -1705,7 +1712,7 @@
         <v>1</v>
       </c>
       <c r="G16">
-        <f>1-F16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H16" t="s">
@@ -1722,7 +1729,7 @@
       </c>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="B17" s="6" t="s">
         <v>25</v>
       </c>
       <c r="C17" s="3" t="s">
@@ -1738,7 +1745,7 @@
         <v>1</v>
       </c>
       <c r="G17">
-        <f>1-F17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H17" t="s">
@@ -1755,7 +1762,7 @@
       </c>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="B18" s="6" t="s">
         <v>44</v>
       </c>
       <c r="C18" s="3" t="s">
@@ -1771,7 +1778,7 @@
         <v>1</v>
       </c>
       <c r="G18">
-        <f>1-F18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H18" t="s">
@@ -1788,7 +1795,7 @@
       </c>
     </row>
     <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="B19" s="6" t="s">
         <v>45</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1804,7 +1811,7 @@
         <v>1</v>
       </c>
       <c r="G19">
-        <f>1-F19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H19" t="s">
@@ -1821,7 +1828,7 @@
       </c>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="B20" s="6" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -1837,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="G20">
-        <f>1-F20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H20" t="s">
@@ -1854,7 +1861,7 @@
       </c>
     </row>
     <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="B21" s="6" t="s">
         <v>51</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -1870,7 +1877,7 @@
         <v>1</v>
       </c>
       <c r="G21">
-        <f>1-F21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H21" t="s">
@@ -1887,7 +1894,7 @@
       </c>
     </row>
     <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="B22" s="6" t="s">
         <v>53</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -1903,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="G22">
-        <f>1-F22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H22" t="s">
@@ -1920,7 +1927,7 @@
       </c>
     </row>
     <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="B23" s="6" t="s">
         <v>60</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -1936,7 +1943,7 @@
         <v>1</v>
       </c>
       <c r="G23">
-        <f>1-F23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H23" t="s">
@@ -1953,7 +1960,7 @@
       </c>
     </row>
     <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="B24" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -1969,7 +1976,7 @@
         <v>1</v>
       </c>
       <c r="G24">
-        <f>1-F24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H24" t="s">
@@ -1986,7 +1993,7 @@
       </c>
     </row>
     <row r="25" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="B25" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -2002,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="G25">
-        <f>1-F25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H25" t="s">
@@ -2019,7 +2026,7 @@
       </c>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="B26" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -2035,7 +2042,7 @@
         <v>1</v>
       </c>
       <c r="G26">
-        <f>1-F26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H26" t="s">
@@ -2052,7 +2059,7 @@
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="B27" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -2068,7 +2075,7 @@
         <v>1</v>
       </c>
       <c r="G27">
-        <f>1-F27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H27" t="s">
@@ -2085,7 +2092,7 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="B28" s="6" t="s">
         <v>112</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -2101,7 +2108,7 @@
         <v>1</v>
       </c>
       <c r="G28">
-        <f>1-F28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H28" t="s">
@@ -2118,7 +2125,7 @@
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
         <v>113</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -2134,7 +2141,7 @@
         <v>1</v>
       </c>
       <c r="G29">
-        <f>1-F29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H29" t="s">
@@ -2151,7 +2158,7 @@
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="B30" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -2167,7 +2174,7 @@
         <v>1</v>
       </c>
       <c r="G30">
-        <f>1-F30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H30" t="s">
@@ -2184,7 +2191,7 @@
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="B31" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -2200,7 +2207,7 @@
         <v>1</v>
       </c>
       <c r="G31">
-        <f>1-F31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H31" t="s">
@@ -2217,7 +2224,7 @@
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="B32" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -2233,7 +2240,7 @@
         <v>1</v>
       </c>
       <c r="G32">
-        <f>1-F32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H32" t="s">
@@ -2250,7 +2257,7 @@
       </c>
     </row>
     <row r="33" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+      <c r="B33" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C33" s="3" t="s">
@@ -2266,7 +2273,7 @@
         <v>1</v>
       </c>
       <c r="G33">
-        <f>1-F33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H33" t="s">
@@ -2283,7 +2290,7 @@
       </c>
     </row>
     <row r="34" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+      <c r="B34" s="6" t="s">
         <v>3</v>
       </c>
       <c r="C34" s="3" t="s">
@@ -2299,7 +2306,7 @@
         <v>1</v>
       </c>
       <c r="G34">
-        <f>1-F34</f>
+        <f t="shared" ref="G34:G65" si="1">1-F34</f>
         <v>0</v>
       </c>
       <c r="H34" t="s">
@@ -2316,7 +2323,7 @@
       </c>
     </row>
     <row r="35" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="B35" s="6" t="s">
         <v>6</v>
       </c>
       <c r="C35" s="3" t="s">
@@ -2332,7 +2339,7 @@
         <v>1</v>
       </c>
       <c r="G35">
-        <f>1-F35</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H35" t="s">
@@ -2349,7 +2356,7 @@
       </c>
     </row>
     <row r="36" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="B36" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="3" t="s">
@@ -2365,7 +2372,7 @@
         <v>1</v>
       </c>
       <c r="G36">
-        <f>1-F36</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H36" t="s">
@@ -2382,7 +2389,7 @@
       </c>
     </row>
     <row r="37" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+      <c r="B37" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
@@ -2398,7 +2405,7 @@
         <v>1</v>
       </c>
       <c r="G37">
-        <f>1-F37</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H37" t="s">
@@ -2415,7 +2422,7 @@
       </c>
     </row>
     <row r="38" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+      <c r="B38" s="6" t="s">
         <v>15</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -2431,7 +2438,7 @@
         <v>1</v>
       </c>
       <c r="G38">
-        <f>1-F38</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H38" t="s">
@@ -2448,7 +2455,7 @@
       </c>
     </row>
     <row r="39" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+      <c r="B39" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -2464,7 +2471,7 @@
         <v>1</v>
       </c>
       <c r="G39">
-        <f>1-F39</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H39" t="s">
@@ -2481,7 +2488,7 @@
       </c>
     </row>
     <row r="40" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+      <c r="B40" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -2497,7 +2504,7 @@
         <v>1</v>
       </c>
       <c r="G40">
-        <f>1-F40</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H40" t="s">
@@ -2514,7 +2521,7 @@
       </c>
     </row>
     <row r="41" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+      <c r="B41" s="6" t="s">
         <v>22</v>
       </c>
       <c r="C41" s="3" t="s">
@@ -2530,7 +2537,7 @@
         <v>1</v>
       </c>
       <c r="G41">
-        <f>1-F41</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H41" t="s">
@@ -2547,7 +2554,7 @@
       </c>
     </row>
     <row r="42" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+      <c r="B42" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C42" s="3" t="s">
@@ -2563,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="G42">
-        <f>1-F42</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H42" t="s">
@@ -2580,7 +2587,7 @@
       </c>
     </row>
     <row r="43" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+      <c r="B43" s="6" t="s">
         <v>29</v>
       </c>
       <c r="C43" s="3" t="s">
@@ -2596,7 +2603,7 @@
         <v>1</v>
       </c>
       <c r="G43">
-        <f>1-F43</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H43" t="s">
@@ -2613,7 +2620,7 @@
       </c>
     </row>
     <row r="44" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+      <c r="B44" s="6" t="s">
         <v>35</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -2629,7 +2636,7 @@
         <v>1</v>
       </c>
       <c r="G44">
-        <f>1-F44</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H44" t="s">
@@ -2646,7 +2653,7 @@
       </c>
     </row>
     <row r="45" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+      <c r="B45" s="6" t="s">
         <v>46</v>
       </c>
       <c r="C45" s="3" t="s">
@@ -2662,7 +2669,7 @@
         <v>1</v>
       </c>
       <c r="G45">
-        <f>1-F45</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H45" t="s">
@@ -2679,7 +2686,7 @@
       </c>
     </row>
     <row r="46" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+      <c r="B46" s="6" t="s">
         <v>47</v>
       </c>
       <c r="C46" s="3" t="s">
@@ -2695,7 +2702,7 @@
         <v>1</v>
       </c>
       <c r="G46">
-        <f>1-F46</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H46" t="s">
@@ -2712,7 +2719,7 @@
       </c>
     </row>
     <row r="47" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+      <c r="B47" s="6" t="s">
         <v>48</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2728,7 +2735,7 @@
         <v>1</v>
       </c>
       <c r="G47">
-        <f>1-F47</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H47" t="s">
@@ -2745,7 +2752,7 @@
       </c>
     </row>
     <row r="48" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+      <c r="B48" s="6" t="s">
         <v>52</v>
       </c>
       <c r="C48" s="3" t="s">
@@ -2761,7 +2768,7 @@
         <v>1</v>
       </c>
       <c r="G48">
-        <f>1-F48</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H48" t="s">
@@ -2778,7 +2785,7 @@
       </c>
     </row>
     <row r="49" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+      <c r="B49" s="6" t="s">
         <v>55</v>
       </c>
       <c r="C49" s="3" t="s">
@@ -2794,7 +2801,7 @@
         <v>1</v>
       </c>
       <c r="G49">
-        <f>1-F49</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H49" t="s">
@@ -2811,7 +2818,7 @@
       </c>
     </row>
     <row r="50" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+      <c r="B50" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -2827,7 +2834,7 @@
         <v>1</v>
       </c>
       <c r="G50">
-        <f>1-F50</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H50" t="s">
@@ -2844,7 +2851,7 @@
       </c>
     </row>
     <row r="51" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+      <c r="B51" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C51" s="3" t="s">
@@ -2860,7 +2867,7 @@
         <v>1</v>
       </c>
       <c r="G51">
-        <f>1-F51</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H51" t="s">
@@ -2877,7 +2884,7 @@
       </c>
     </row>
     <row r="52" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+      <c r="B52" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -2893,7 +2900,7 @@
         <v>1</v>
       </c>
       <c r="G52">
-        <f>1-F52</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H52" t="s">
@@ -2910,7 +2917,7 @@
       </c>
     </row>
     <row r="53" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+      <c r="B53" s="6" t="s">
         <v>117</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -2926,7 +2933,7 @@
         <v>1</v>
       </c>
       <c r="G53">
-        <f>1-F53</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H53" t="s">
@@ -2943,7 +2950,7 @@
       </c>
     </row>
     <row r="54" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="B54" s="6" t="s">
         <v>119</v>
       </c>
       <c r="C54" s="3" t="s">
@@ -2959,7 +2966,7 @@
         <v>1</v>
       </c>
       <c r="G54">
-        <f>1-F54</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H54" t="s">
@@ -2976,7 +2983,7 @@
       </c>
     </row>
     <row r="55" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+      <c r="B55" s="6" t="s">
         <v>121</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -2992,7 +2999,7 @@
         <v>1</v>
       </c>
       <c r="G55">
-        <f>1-F55</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H55" t="s">
@@ -3009,7 +3016,7 @@
       </c>
     </row>
     <row r="56" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+      <c r="B56" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C56" s="3" t="s">
@@ -3025,7 +3032,7 @@
         <v>1</v>
       </c>
       <c r="G56">
-        <f>1-F56</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H56" t="s">
@@ -3042,7 +3049,7 @@
       </c>
     </row>
     <row r="57" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+      <c r="B57" s="6" t="s">
         <v>125</v>
       </c>
       <c r="C57" s="3" t="s">
@@ -3058,7 +3065,7 @@
         <v>1</v>
       </c>
       <c r="G57">
-        <f>1-F57</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H57" t="s">
@@ -3075,7 +3082,7 @@
       </c>
     </row>
     <row r="58" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+      <c r="B58" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C58" s="3" t="s">
@@ -3091,7 +3098,7 @@
         <v>1</v>
       </c>
       <c r="G58">
-        <f>1-F58</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H58" t="s">
@@ -3108,7 +3115,7 @@
       </c>
     </row>
     <row r="59" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+      <c r="B59" s="6" t="s">
         <v>104</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -3124,7 +3131,7 @@
         <v>1</v>
       </c>
       <c r="G59">
-        <f>1-F59</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="H59" t="s">
@@ -3141,7 +3148,7 @@
       </c>
     </row>
     <row r="60" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+      <c r="B60" s="6" t="s">
         <v>67</v>
       </c>
       <c r="C60" s="3" t="s">
@@ -3157,7 +3164,7 @@
         <v>0</v>
       </c>
       <c r="G60">
-        <f>1-F60</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H60" t="s">
@@ -3174,7 +3181,7 @@
       </c>
     </row>
     <row r="61" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="B61" s="6" t="s">
         <v>70</v>
       </c>
       <c r="C61" s="3" t="s">
@@ -3190,7 +3197,7 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <f>1-F61</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H61" t="s">
@@ -3207,7 +3214,7 @@
       </c>
     </row>
     <row r="62" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+      <c r="B62" s="6" t="s">
         <v>72</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -3223,7 +3230,7 @@
         <v>0</v>
       </c>
       <c r="G62">
-        <f>1-F62</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H62" t="s">
@@ -3240,7 +3247,7 @@
       </c>
     </row>
     <row r="63" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+      <c r="B63" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -3256,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="G63">
-        <f>1-F63</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H63" t="s">
@@ -3273,7 +3280,7 @@
       </c>
     </row>
     <row r="64" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+      <c r="B64" s="6" t="s">
         <v>76</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -3289,7 +3296,7 @@
         <v>0</v>
       </c>
       <c r="G64">
-        <f>1-F64</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H64" t="s">
@@ -3306,7 +3313,7 @@
       </c>
     </row>
     <row r="65" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+      <c r="B65" s="6" t="s">
         <v>78</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -3322,7 +3329,7 @@
         <v>0</v>
       </c>
       <c r="G65">
-        <f>1-F65</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="H65" t="s">
@@ -3339,7 +3346,7 @@
       </c>
     </row>
     <row r="66" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B66" t="s">
+      <c r="B66" s="6" t="s">
         <v>83</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -3355,7 +3362,7 @@
         <v>1</v>
       </c>
       <c r="G66">
-        <f>1-F66</f>
+        <f t="shared" ref="G66:G97" si="2">1-F66</f>
         <v>0</v>
       </c>
       <c r="H66" t="s">
@@ -3372,7 +3379,7 @@
       </c>
     </row>
     <row r="67" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
+      <c r="B67" s="6" t="s">
         <v>145</v>
       </c>
       <c r="C67" s="3" t="s">
@@ -3388,7 +3395,7 @@
         <v>1</v>
       </c>
       <c r="G67">
-        <f>1-F67</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H67" t="s">
@@ -3405,7 +3412,7 @@
       </c>
     </row>
     <row r="68" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
+      <c r="B68" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C68" s="3" t="s">
@@ -3421,7 +3428,7 @@
         <v>1</v>
       </c>
       <c r="G68">
-        <f>1-F68</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H68" t="s">
@@ -3438,7 +3445,7 @@
       </c>
     </row>
     <row r="69" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B69" t="s">
+      <c r="B69" s="6" t="s">
         <v>64</v>
       </c>
       <c r="C69" s="3" t="s">
@@ -3454,7 +3461,7 @@
         <v>0</v>
       </c>
       <c r="G69">
-        <f>1-F69</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H69" t="s">
@@ -3471,7 +3478,7 @@
       </c>
     </row>
     <row r="70" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B70" t="s">
+      <c r="B70" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -3487,7 +3494,7 @@
         <v>1</v>
       </c>
       <c r="G70">
-        <f>1-F70</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H70" t="s">
@@ -3504,7 +3511,7 @@
       </c>
     </row>
     <row r="71" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B71" t="s">
+      <c r="B71" s="6" t="s">
         <v>103</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -3520,7 +3527,7 @@
         <v>1</v>
       </c>
       <c r="G71">
-        <f>1-F71</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H71" t="s">
@@ -3537,7 +3544,7 @@
       </c>
     </row>
     <row r="72" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B72" t="s">
+      <c r="B72" s="6" t="s">
         <v>116</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -3553,7 +3560,7 @@
         <v>1</v>
       </c>
       <c r="G72">
-        <f>1-F72</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H72" t="s">
@@ -3570,7 +3577,7 @@
       </c>
     </row>
     <row r="73" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B73" t="s">
+      <c r="B73" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -3586,7 +3593,7 @@
         <v>1</v>
       </c>
       <c r="G73">
-        <f>1-F73</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H73" t="s">
@@ -3603,7 +3610,7 @@
       </c>
     </row>
     <row r="74" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B74" t="s">
+      <c r="B74" s="6" t="s">
         <v>120</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -3619,7 +3626,7 @@
         <v>1</v>
       </c>
       <c r="G74">
-        <f>1-F74</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H74" t="s">
@@ -3636,7 +3643,7 @@
       </c>
     </row>
     <row r="75" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B75" t="s">
+      <c r="B75" s="6" t="s">
         <v>122</v>
       </c>
       <c r="C75" s="3" t="s">
@@ -3652,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="G75">
-        <f>1-F75</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H75" t="s">
@@ -3669,7 +3676,7 @@
       </c>
     </row>
     <row r="76" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B76" t="s">
+      <c r="B76" s="6" t="s">
         <v>124</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -3685,7 +3692,7 @@
         <v>1</v>
       </c>
       <c r="G76">
-        <f>1-F76</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H76" t="s">
@@ -3702,7 +3709,7 @@
       </c>
     </row>
     <row r="77" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B77" t="s">
+      <c r="B77" s="6" t="s">
         <v>126</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -3718,7 +3725,7 @@
         <v>1</v>
       </c>
       <c r="G77">
-        <f>1-F77</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H77" t="s">
@@ -3735,7 +3742,7 @@
       </c>
     </row>
     <row r="78" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B78" t="s">
+      <c r="B78" s="6" t="s">
         <v>128</v>
       </c>
       <c r="C78" s="3" t="s">
@@ -3751,7 +3758,7 @@
         <v>1</v>
       </c>
       <c r="G78">
-        <f>1-F78</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H78" t="s">
@@ -3768,7 +3775,7 @@
       </c>
     </row>
     <row r="79" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
+      <c r="B79" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C79" s="3">
@@ -3784,7 +3791,7 @@
         <v>1</v>
       </c>
       <c r="G79">
-        <f>1-F79</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H79" t="s">
@@ -3801,7 +3808,7 @@
       </c>
     </row>
     <row r="80" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
+      <c r="B80" s="6" t="s">
         <v>80</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -3817,7 +3824,7 @@
         <v>0</v>
       </c>
       <c r="G80">
-        <f>1-F80</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H80" t="s">
@@ -3834,7 +3841,7 @@
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B81" t="s">
+      <c r="B81" s="6" t="s">
         <v>57</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -3850,7 +3857,7 @@
         <v>1</v>
       </c>
       <c r="G81">
-        <f>1-F81</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H81" t="s">
@@ -3867,7 +3874,7 @@
       </c>
     </row>
     <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82" t="s">
+      <c r="B82" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -3883,7 +3890,7 @@
         <v>1</v>
       </c>
       <c r="G82">
-        <f>1-F82</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H82" t="s">
@@ -3900,7 +3907,7 @@
       </c>
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B83" t="s">
+      <c r="B83" s="6" t="s">
         <v>225</v>
       </c>
       <c r="C83" s="3" t="s">
@@ -3916,7 +3923,7 @@
         <v>1</v>
       </c>
       <c r="G83">
-        <f>1-F83</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H83" t="s">
@@ -3933,7 +3940,7 @@
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B84" t="s">
+      <c r="B84" s="6" t="s">
         <v>148</v>
       </c>
       <c r="C84" s="3" t="s">
@@ -3949,7 +3956,7 @@
         <v>1</v>
       </c>
       <c r="G84">
-        <f>1-F84</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H84" t="s">
@@ -3966,7 +3973,7 @@
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B85" t="s">
+      <c r="B85" s="6" t="s">
         <v>36</v>
       </c>
       <c r="C85" s="3" t="s">
@@ -3982,7 +3989,7 @@
         <v>1</v>
       </c>
       <c r="G85">
-        <f>1-F85</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="H85" t="s">
@@ -3999,7 +4006,7 @@
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
+      <c r="B86" s="6" t="s">
         <v>61</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -4015,7 +4022,7 @@
         <v>0</v>
       </c>
       <c r="G86">
-        <f>1-F86</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="H86" t="s">
@@ -4032,7 +4039,7 @@
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
+      <c r="B87" s="6" t="s">
         <v>86</v>
       </c>
       <c r="C87" s="3" t="s">
@@ -4059,7 +4066,7 @@
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B88" t="s">
+      <c r="B88" s="6" t="s">
         <v>89</v>
       </c>
       <c r="C88" s="3" t="s">
@@ -4086,7 +4093,7 @@
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B89" t="s">
+      <c r="B89" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C89" s="3" t="s">
@@ -4113,7 +4120,7 @@
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B90" t="s">
+      <c r="B90" s="6" t="s">
         <v>95</v>
       </c>
       <c r="C90" s="3" t="s">
@@ -4140,7 +4147,7 @@
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B91" t="s">
+      <c r="B91" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C91" s="3" t="s">
@@ -4167,7 +4174,7 @@
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B92" t="s">
+      <c r="B92" s="6" t="s">
         <v>130</v>
       </c>
       <c r="C92" s="3" t="s">
@@ -4200,7 +4207,7 @@
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
+      <c r="B93" s="6" t="s">
         <v>133</v>
       </c>
       <c r="C93" s="3" t="s">
@@ -4233,7 +4240,7 @@
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B94" t="s">
+      <c r="B94" s="6" t="s">
         <v>139</v>
       </c>
       <c r="C94" s="3" t="s">
@@ -4266,7 +4273,7 @@
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B95" t="s">
+      <c r="B95" s="6" t="s">
         <v>142</v>
       </c>
       <c r="C95" s="3" t="s">

</xml_diff>